<commit_message>
feat: nguyên liệu, ncc, món ăn
</commit_message>
<xml_diff>
--- a/upload/emps.xlsx
+++ b/upload/emps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Master\2. CSDLNC\BTL\BTL.Web\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D78220-8ED6-4A56-87F5-5C3B3CC56E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A0AA47-5465-4FBF-BF75-D27FAE305F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{39C9C632-DC3E-4A47-8DD7-1923FC113CAB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="62">
   <si>
     <t>STT</t>
   </si>
@@ -211,9 +211,6 @@
   </si>
   <si>
     <t>Mã nhân viên</t>
-  </si>
-  <si>
-    <t>NV1005</t>
   </si>
 </sst>
 </file>
@@ -608,7 +605,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -647,9 +644,6 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>